<commit_message>
Adding additional analytics to TestDashboard.xlsx.
</commit_message>
<xml_diff>
--- a/documentation/TestDashboard.xlsx
+++ b/documentation/TestDashboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14640" windowHeight="6960" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14640" windowHeight="6960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Calendar" sheetId="2" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="Session Report" sheetId="7" r:id="rId6"/>
     <sheet name="Completed" sheetId="3" r:id="rId7"/>
     <sheet name="Velocity" sheetId="5" r:id="rId8"/>
+    <sheet name="Allocation" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="bug" localSheetId="4">'Session Summary'!$A$21</definedName>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="200">
   <si>
     <t>Testing Dashboard</t>
   </si>
@@ -877,13 +878,44 @@
 T - testing
 I - investigate</t>
   </si>
+  <si>
+    <t>Allocation Report</t>
+  </si>
+  <si>
+    <t>Scripting</t>
+  </si>
+  <si>
+    <t>Analysis</t>
+  </si>
+  <si>
+    <t>Automated Test</t>
+  </si>
+  <si>
+    <t>Manual Test</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>Automating</t>
+  </si>
+  <si>
+    <t>Feature Specification</t>
+  </si>
+  <si>
+    <t>Total Hours</t>
+  </si>
+  <si>
+    <t>Total %</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1124,7 +1156,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1224,20 +1256,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1254,18 +1289,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1275,11 +1298,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1304,6 +1333,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1337,6 +1372,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1485,12 +1529,12 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:shape val="box"/>
-        <c:axId val="90789376"/>
-        <c:axId val="90790912"/>
+        <c:axId val="125187968"/>
+        <c:axId val="125189504"/>
         <c:axId val="0"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="90789376"/>
+        <c:axId val="125187968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1499,7 +1543,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90790912"/>
+        <c:crossAx val="125189504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1507,7 +1551,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90790912"/>
+        <c:axId val="125189504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1518,7 +1562,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90789376"/>
+        <c:crossAx val="125187968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1757,11 +1801,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="90977792"/>
-        <c:axId val="90979328"/>
+        <c:axId val="125380096"/>
+        <c:axId val="125381632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90977792"/>
+        <c:axId val="125380096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1770,7 +1814,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90979328"/>
+        <c:crossAx val="125381632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1778,7 +1822,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90979328"/>
+        <c:axId val="125381632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1789,7 +1833,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90977792"/>
+        <c:crossAx val="125380096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1798,6 +1842,2196 @@
       <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="30"/>
+      <c:rotY val="0"/>
+      <c:rAngAx val="0"/>
+      <c:perspective val="30"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Allocation!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Allocation Report</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$3:$I$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Hello2</c:v>
+          </c:tx>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$4:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$5:$I$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$6:$I$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$7:$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$8:$I$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$9:$I$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$10:$I$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$12:$I$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$13:$I$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$14:$I$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$15:$I$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$16:$I$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$17:$I$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$18:$I$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$19:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$20:$I$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$21:$I$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$22:$I$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$23:$I$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="21"/>
+          <c:order val="21"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$24:$I$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="22"/>
+          <c:order val="22"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$25:$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="23"/>
+          <c:order val="23"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$26:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="24"/>
+          <c:order val="24"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$27:$I$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="25"/>
+          <c:order val="25"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$28:$I$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="26"/>
+          <c:order val="26"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$29:$I$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="27"/>
+          <c:order val="27"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$30:$I$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="28"/>
+          <c:order val="28"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$31:$I$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="29"/>
+          <c:order val="29"/>
+          <c:explosion val="25"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Allocation!$B$2:$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>Feature Specification</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Execution</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Scripting</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Automating</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Analysis</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Maintenance</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Allocation!$B$32:$I$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
@@ -1860,6 +4094,41 @@
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2171,7 +4440,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2181,14 +4450,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="34" t="s">
@@ -2218,19 +4487,19 @@
       <c r="A3" s="10">
         <v>1</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="47" t="s">
+      <c r="C3" s="48" t="s">
         <v>27</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E3" s="45" t="s">
+      <c r="E3" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="48" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2238,39 +4507,39 @@
       <c r="A4" s="10">
         <v>2</v>
       </c>
-      <c r="B4" s="46"/>
-      <c r="C4" s="47"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
-      <c r="F4" s="47"/>
+      <c r="B4" s="50"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="50"/>
+      <c r="E4" s="50"/>
+      <c r="F4" s="48"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
-      <c r="B5" s="50"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="47"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="48"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
-      <c r="B6" s="47" t="s">
+      <c r="B6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="47" t="s">
+      <c r="C6" s="48" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="F6" s="47" t="s">
+      <c r="F6" s="48" t="s">
         <v>29</v>
       </c>
     </row>
@@ -2278,37 +4547,37 @@
       <c r="A7" s="10">
         <v>5</v>
       </c>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="50"/>
+      <c r="E7" s="50"/>
+      <c r="F7" s="48"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="10">
         <v>6</v>
       </c>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="46"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="47"/>
+      <c r="B8" s="48"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="48"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>7</v>
       </c>
-      <c r="B9" s="47"/>
-      <c r="C9" s="45" t="s">
+      <c r="B9" s="48"/>
+      <c r="C9" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="F9" s="47" t="s">
+      <c r="F9" s="48" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2316,57 +4585,57 @@
       <c r="A10" s="10">
         <v>8</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="47"/>
+      <c r="B10" s="48"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="48"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="10">
         <v>9</v>
       </c>
-      <c r="B11" s="47"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="47"/>
+      <c r="B11" s="48"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="48"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>10</v>
       </c>
-      <c r="B12" s="47"/>
-      <c r="C12" s="47" t="s">
+      <c r="B12" s="48"/>
+      <c r="C12" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="D12" s="47" t="s">
+      <c r="D12" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="E12" s="47" t="s">
+      <c r="E12" s="48" t="s">
         <v>99</v>
       </c>
-      <c r="F12" s="47"/>
+      <c r="F12" s="48"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="10">
         <v>11</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="47"/>
-      <c r="D13" s="47"/>
-      <c r="E13" s="47"/>
-      <c r="F13" s="47"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
+      <c r="F13" s="48"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="10">
         <v>12</v>
       </c>
-      <c r="B14" s="47"/>
-      <c r="C14" s="47"/>
-      <c r="D14" s="47"/>
-      <c r="E14" s="47"/>
-      <c r="F14" s="47"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="48"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
+      <c r="F14" s="48"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -2379,6 +4648,8 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F6:F8"/>
+    <mergeCell ref="F9:F14"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B6:B14"/>
     <mergeCell ref="C9:C11"/>
@@ -2395,8 +4666,6 @@
     <mergeCell ref="E12:E14"/>
     <mergeCell ref="E6:E8"/>
     <mergeCell ref="F3:F5"/>
-    <mergeCell ref="F6:F8"/>
-    <mergeCell ref="F9:F14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2431,31 +4700,31 @@
       <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="53" t="s">
+      <c r="G2" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="51" t="s">
+      <c r="I2" s="52" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="52" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2463,15 +4732,15 @@
       <c r="A3" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="52"/>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="52"/>
-      <c r="I3" s="52"/>
-      <c r="J3" s="52"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
@@ -2745,17 +5014,17 @@
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -2878,55 +5147,55 @@
       <c r="C16" s="1"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="56" t="s">
+      <c r="A17" s="59" t="s">
         <v>177</v>
       </c>
-      <c r="B17" s="57"/>
+      <c r="B17" s="60"/>
       <c r="C17" s="17" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="B18" s="57"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="17" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="B19" s="57"/>
+      <c r="B19" s="60"/>
       <c r="C19" s="17" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="60" t="s">
+      <c r="A20" s="57" t="s">
         <v>176</v>
       </c>
-      <c r="B20" s="61"/>
+      <c r="B20" s="58"/>
       <c r="C20" s="17" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="56" t="s">
+      <c r="A21" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="B21" s="57"/>
+      <c r="B21" s="60"/>
       <c r="C21" s="17" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="56" t="s">
+      <c r="A22" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="B22" s="57"/>
+      <c r="B22" s="60"/>
       <c r="C22" s="17" t="s">
         <v>87</v>
       </c>
@@ -3006,42 +5275,42 @@
       <c r="A36" s="4"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="B37" s="58"/>
+      <c r="B37" s="62"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="55" t="s">
+      <c r="A38" s="61" t="s">
         <v>186</v>
       </c>
-      <c r="B38" s="55"/>
+      <c r="B38" s="61"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" s="55" t="s">
+      <c r="A39" s="61" t="s">
         <v>187</v>
       </c>
-      <c r="B39" s="55"/>
+      <c r="B39" s="61"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="61" t="s">
         <v>188</v>
       </c>
-      <c r="B40" s="55"/>
+      <c r="B40" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
     <mergeCell ref="A40:B40"/>
     <mergeCell ref="A21:B21"/>
     <mergeCell ref="A22:B22"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A38:B38"/>
     <mergeCell ref="A39:B39"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3051,7 +5320,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
@@ -3069,129 +5338,129 @@
       <c r="A1" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
+      <c r="B2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="65"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="66"/>
+      <c r="B3" s="63"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="71" t="s">
+      <c r="C4" s="64"/>
+      <c r="D4" s="65"/>
+      <c r="E4" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-      <c r="L4" s="71"/>
+      <c r="F4" s="70"/>
+      <c r="G4" s="70"/>
+      <c r="H4" s="70"/>
+      <c r="I4" s="70"/>
+      <c r="J4" s="70"/>
+      <c r="K4" s="70"/>
+      <c r="L4" s="70"/>
     </row>
     <row r="5" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="67" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="69"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
-      <c r="K5" s="71"/>
-      <c r="L5" s="71"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
     </row>
     <row r="6" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="64" t="s">
+      <c r="B6" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="C6" s="65"/>
-      <c r="D6" s="66"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
+      <c r="C6" s="64"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="70"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
       <c r="O6" s="25"/>
       <c r="P6" s="25"/>
       <c r="Q6" s="25"/>
       <c r="R6" s="9"/>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67" t="s">
+      <c r="A7" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="51" t="s">
+      <c r="B7" s="66"/>
+      <c r="C7" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="E7" s="51" t="s">
+      <c r="E7" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="67" t="s">
+      <c r="F7" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="53" t="s">
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="54" t="s">
         <v>73</v>
       </c>
-      <c r="J7" s="53" t="s">
+      <c r="J7" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="K7" s="51" t="s">
+      <c r="K7" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="51" t="s">
+      <c r="L7" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="N7" s="62" t="s">
+      <c r="N7" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="O7" s="63" t="s">
+      <c r="O7" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="P7" s="63" t="s">
+      <c r="P7" s="72" t="s">
         <v>40</v>
       </c>
-      <c r="Q7" s="63" t="s">
+      <c r="Q7" s="72" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3202,9 +5471,9 @@
       <c r="B8" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
       <c r="F8" s="23" t="s">
         <v>72</v>
       </c>
@@ -3214,14 +5483,14 @@
       <c r="H8" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="54"/>
-      <c r="J8" s="54"/>
-      <c r="K8" s="52"/>
-      <c r="L8" s="52"/>
-      <c r="N8" s="62"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="63"/>
-      <c r="Q8" s="63"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="55"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="N8" s="71"/>
+      <c r="O8" s="72"/>
+      <c r="P8" s="72"/>
+      <c r="Q8" s="72"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
@@ -3636,6 +5905,12 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
+    <mergeCell ref="P7:P8"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="K7:K8"/>
+    <mergeCell ref="L7:L8"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="F7:H7"/>
     <mergeCell ref="I7:I8"/>
@@ -3650,12 +5925,6 @@
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="E4:L6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
-    <mergeCell ref="P7:P8"/>
-    <mergeCell ref="Q7:Q8"/>
-    <mergeCell ref="K7:K8"/>
-    <mergeCell ref="L7:L8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3690,7 +5959,7 @@
   <dimension ref="A2:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4173,8 +6442,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4206,10 +6475,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="76" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="75"/>
+      <c r="B2" s="76"/>
       <c r="D2" t="s">
         <v>155</v>
       </c>
@@ -4224,10 +6493,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="80" t="s">
+      <c r="A3" s="81" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="81"/>
+      <c r="B3" s="82"/>
       <c r="D3" t="s">
         <v>156</v>
       </c>
@@ -4239,10 +6508,10 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="77" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="77"/>
+      <c r="B4" s="78"/>
       <c r="D4" t="s">
         <v>125</v>
       </c>
@@ -4312,10 +6581,10 @@
       <c r="B11" s="1"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="77" t="s">
         <v>164</v>
       </c>
-      <c r="B12" s="77"/>
+      <c r="B12" s="78"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="26" t="s">
@@ -4372,28 +6641,28 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="77" t="s">
+      <c r="B20" s="78" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="78" t="s">
+      <c r="A21" s="79" t="s">
         <v>109</v>
       </c>
-      <c r="B21" s="79"/>
+      <c r="B21" s="80"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="77"/>
+      <c r="B22" s="78"/>
     </row>
     <row r="23" spans="1:2" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
-      <c r="B23" s="55"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
@@ -4440,46 +6709,46 @@
       <c r="B31" s="1"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="76" t="s">
+      <c r="A33" s="77" t="s">
         <v>119</v>
       </c>
-      <c r="B33" s="77"/>
+      <c r="B33" s="78"/>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="73" t="s">
+      <c r="A34" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="B34" s="74"/>
+      <c r="B34" s="75"/>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="73" t="s">
+      <c r="A35" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="B35" s="74"/>
+      <c r="B35" s="75"/>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="73" t="s">
+      <c r="A36" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="B36" s="74"/>
+      <c r="B36" s="75"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" s="73" t="s">
+      <c r="A37" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="B37" s="74"/>
+      <c r="B37" s="75"/>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" s="73" t="s">
+      <c r="A38" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="B38" s="74"/>
+      <c r="B38" s="75"/>
     </row>
     <row r="39" spans="1:2" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="72" t="s">
+      <c r="A39" s="73" t="s">
         <v>189</v>
       </c>
-      <c r="B39" s="72"/>
+      <c r="B39" s="73"/>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="43"/>
@@ -4532,7 +6801,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4544,13 +6813,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="48" t="s">
+      <c r="A1" s="46" t="s">
         <v>123</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
@@ -4667,8 +6936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4678,12 +6947,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
+      <c r="B1" s="83"/>
+      <c r="C1" s="83"/>
+      <c r="D1" s="83"/>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="31" t="s">
@@ -5042,4 +7311,1085 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="47"/>
+      <c r="C1" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="76"/>
+      <c r="E1" s="78"/>
+      <c r="F1" s="77" t="s">
+        <v>193</v>
+      </c>
+      <c r="G1" s="76"/>
+      <c r="H1" s="76"/>
+      <c r="I1" s="78"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="B2" s="45" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="D2" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="F2" s="45" t="s">
+        <v>191</v>
+      </c>
+      <c r="G2" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="H2" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="I2" s="45" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <f>Dashboard!B1</f>
+        <v>41709</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <f>A3+1</f>
+        <v>41710</v>
+      </c>
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="21">
+        <f t="shared" ref="A5:A32" si="0">A4+1</f>
+        <v>41711</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="21">
+        <f t="shared" si="0"/>
+        <v>41712</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <f t="shared" si="0"/>
+        <v>41713</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <f t="shared" si="0"/>
+        <v>41714</v>
+      </c>
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="21">
+        <f t="shared" si="0"/>
+        <v>41715</v>
+      </c>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="21">
+        <f t="shared" si="0"/>
+        <v>41716</v>
+      </c>
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="21">
+        <f t="shared" si="0"/>
+        <v>41717</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="21">
+        <f t="shared" si="0"/>
+        <v>41718</v>
+      </c>
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="21">
+        <f t="shared" si="0"/>
+        <v>41719</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>0</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1">
+        <v>0</v>
+      </c>
+      <c r="I13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="21">
+        <f t="shared" si="0"/>
+        <v>41720</v>
+      </c>
+      <c r="B14" s="1">
+        <v>0</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>0</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0</v>
+      </c>
+      <c r="I14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="21">
+        <f t="shared" si="0"/>
+        <v>41721</v>
+      </c>
+      <c r="B15" s="1">
+        <v>0</v>
+      </c>
+      <c r="C15" s="1">
+        <v>0</v>
+      </c>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0</v>
+      </c>
+      <c r="I15" s="1">
+        <v>0</v>
+      </c>
+      <c r="N15" s="84"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="12"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="21">
+        <f t="shared" si="0"/>
+        <v>41722</v>
+      </c>
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>0</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1">
+        <v>0</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="N16" s="84"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="12"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="21">
+        <f t="shared" si="0"/>
+        <v>41723</v>
+      </c>
+      <c r="B17" s="1">
+        <v>0</v>
+      </c>
+      <c r="C17" s="1">
+        <v>0</v>
+      </c>
+      <c r="D17" s="1">
+        <v>0</v>
+      </c>
+      <c r="E17" s="1">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1">
+        <v>0</v>
+      </c>
+      <c r="I17" s="1">
+        <v>0</v>
+      </c>
+      <c r="N17" s="84"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="12"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="21">
+        <f t="shared" si="0"/>
+        <v>41724</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12"/>
+      <c r="P18" s="85"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="21">
+        <f t="shared" si="0"/>
+        <v>41725</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="21">
+        <f t="shared" si="0"/>
+        <v>41726</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0</v>
+      </c>
+      <c r="H20" s="1">
+        <v>0</v>
+      </c>
+      <c r="I20" s="1">
+        <v>0</v>
+      </c>
+      <c r="N20" s="84"/>
+      <c r="O20" s="86"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="86"/>
+      <c r="R20" s="12"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="21">
+        <f t="shared" si="0"/>
+        <v>41727</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>0</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0</v>
+      </c>
+      <c r="N21" s="84"/>
+      <c r="O21" s="86"/>
+      <c r="P21" s="12"/>
+      <c r="Q21" s="86"/>
+      <c r="R21" s="12"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A22" s="21">
+        <f t="shared" si="0"/>
+        <v>41728</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1">
+        <v>0</v>
+      </c>
+      <c r="I22" s="1">
+        <v>0</v>
+      </c>
+      <c r="P22" s="85"/>
+      <c r="R22" s="85"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A23" s="21">
+        <f t="shared" si="0"/>
+        <v>41729</v>
+      </c>
+      <c r="B23" s="1">
+        <v>0</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1">
+        <v>0</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A24" s="21">
+        <f t="shared" si="0"/>
+        <v>41730</v>
+      </c>
+      <c r="B24" s="1">
+        <v>0</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0</v>
+      </c>
+      <c r="I24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A25" s="21">
+        <f t="shared" si="0"/>
+        <v>41731</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0</v>
+      </c>
+      <c r="H25" s="1">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A26" s="21">
+        <f t="shared" si="0"/>
+        <v>41732</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0</v>
+      </c>
+      <c r="H26" s="1">
+        <v>0</v>
+      </c>
+      <c r="I26" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A27" s="21">
+        <f t="shared" si="0"/>
+        <v>41733</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0</v>
+      </c>
+      <c r="H27" s="1">
+        <v>0</v>
+      </c>
+      <c r="I27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="21">
+        <f t="shared" si="0"/>
+        <v>41734</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1">
+        <v>0</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="21">
+        <f t="shared" si="0"/>
+        <v>41735</v>
+      </c>
+      <c r="B29" s="1">
+        <v>0</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>0</v>
+      </c>
+      <c r="F29" s="1">
+        <v>0</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0</v>
+      </c>
+      <c r="H29" s="1">
+        <v>0</v>
+      </c>
+      <c r="I29" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="21">
+        <f t="shared" si="0"/>
+        <v>41736</v>
+      </c>
+      <c r="B30" s="1">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>0</v>
+      </c>
+      <c r="F30" s="1">
+        <v>0</v>
+      </c>
+      <c r="G30" s="1">
+        <v>0</v>
+      </c>
+      <c r="H30" s="1">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="21">
+        <f t="shared" si="0"/>
+        <v>41737</v>
+      </c>
+      <c r="B31" s="1">
+        <v>0</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A32" s="21">
+        <f t="shared" si="0"/>
+        <v>41738</v>
+      </c>
+      <c r="B32" s="1">
+        <v>0</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>0</v>
+      </c>
+      <c r="G32" s="1">
+        <v>0</v>
+      </c>
+      <c r="H32" s="1">
+        <v>0</v>
+      </c>
+      <c r="I32" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" s="88" t="s">
+        <v>198</v>
+      </c>
+      <c r="B33" s="4">
+        <f>SUM(B3:B32)</f>
+        <v>1</v>
+      </c>
+      <c r="C33" s="4">
+        <f t="shared" ref="C33:I33" si="1">SUM(C3:C32)</f>
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E33" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F33" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H33" s="4">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I33" s="4">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="4">
+        <f>SUM(B33:I33)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" s="88" t="s">
+        <v>199</v>
+      </c>
+      <c r="B34" s="87">
+        <f>B33/$J$33</f>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="C34" s="87">
+        <f t="shared" ref="C34:I34" si="2">C33/$J$33</f>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="D34" s="87">
+        <f t="shared" si="2"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="E34" s="87">
+        <f t="shared" si="2"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="F34" s="87">
+        <f t="shared" si="2"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="G34" s="87">
+        <f t="shared" si="2"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="H34" s="87">
+        <f t="shared" si="2"/>
+        <v>0.11764705882352941</v>
+      </c>
+      <c r="I34" s="87">
+        <f t="shared" si="2"/>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="J34" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>